<commit_message>
start sending user id, and adding created by, updated in post/patch/put requests
</commit_message>
<xml_diff>
--- a/documents/timeline/TMML-Changes-Suggested.xlsx
+++ b/documents/timeline/TMML-Changes-Suggested.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B3D5FE-025E-1040-9E2D-3C5D0DC77215}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47BF456-0AC4-DB4B-8AFD-85B16667CB06}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,9 +173,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -224,6 +231,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -245,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -253,21 +266,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -277,12 +296,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -290,22 +307,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <strike val="0"/>
@@ -444,16 +446,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C29DFD18-A044-264A-8D71-38E1691788CC}" name="Table1" displayName="Table1" ref="A1:G23" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C29DFD18-A044-264A-8D71-38E1691788CC}" name="Table1" displayName="Table1" ref="A1:G23" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:G23" xr:uid="{779EFED2-BE53-1A4A-8AF2-57F76D86E31C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{34D16182-3136-D94B-999B-05F2E1E07A8F}" name="Module" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{B7D0AFE2-E6FC-2B49-A2C8-43B223E6AF14}" name="Changes" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{F8C85DE6-5C4E-904B-B8D5-A6AA7357BCB0}" name="Change Type" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{FC13D7FF-763A-E741-82AB-47D466E93BF7}" name="Impact on design" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{2459A3C6-4298-D44D-88FB-DD1D6F2CFA28}" name="Comment" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{DCC083EC-9DE7-614E-9037-C0B7B517DEFC}" name="Status" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{14FBACAC-3368-9448-B5ED-C1BA209E29AC}" name="Man Hours" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{34D16182-3136-D94B-999B-05F2E1E07A8F}" name="Module" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B7D0AFE2-E6FC-2B49-A2C8-43B223E6AF14}" name="Changes" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F8C85DE6-5C4E-904B-B8D5-A6AA7357BCB0}" name="Change Type" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{FC13D7FF-763A-E741-82AB-47D466E93BF7}" name="Impact on design" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{2459A3C6-4298-D44D-88FB-DD1D6F2CFA28}" name="Comment" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{DCC083EC-9DE7-614E-9037-C0B7B517DEFC}" name="Status" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{14FBACAC-3368-9448-B5ED-C1BA209E29AC}" name="Man Hours"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -724,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -778,7 +780,9 @@
         <v>31</v>
       </c>
       <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -797,7 +801,9 @@
         <v>31</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="G3" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -814,7 +820,9 @@
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -833,7 +841,9 @@
         <v>31</v>
       </c>
       <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="14">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -850,7 +860,9 @@
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -869,7 +881,9 @@
         <v>31</v>
       </c>
       <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="G7" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -878,8 +892,8 @@
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>8</v>
+      <c r="C8" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
@@ -888,7 +902,9 @@
         <v>31</v>
       </c>
       <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="G8" s="14">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -907,7 +923,9 @@
         <v>31</v>
       </c>
       <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
@@ -926,7 +944,9 @@
         <v>31</v>
       </c>
       <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="G10" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -943,7 +963,9 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="G11" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
@@ -962,7 +984,9 @@
         <v>31</v>
       </c>
       <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="G12" s="14">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
@@ -979,7 +1003,9 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="G13" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
@@ -998,7 +1024,9 @@
         <v>31</v>
       </c>
       <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="G14" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -1017,7 +1045,9 @@
         <v>31</v>
       </c>
       <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="G15" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
@@ -1030,7 +1060,9 @@
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
       <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="G16" s="14">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -1049,7 +1081,9 @@
         <v>31</v>
       </c>
       <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="G17" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
@@ -1066,7 +1100,9 @@
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="G18" s="14">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
@@ -1085,7 +1121,9 @@
         <v>31</v>
       </c>
       <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="G19" s="14">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
@@ -1104,7 +1142,9 @@
         <v>31</v>
       </c>
       <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="G20" s="14">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
@@ -1123,7 +1163,9 @@
         <v>31</v>
       </c>
       <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="G21" s="14">
+        <v>12</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
@@ -1140,7 +1182,9 @@
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="G22" s="14">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
@@ -1159,7 +1203,9 @@
         <v>31</v>
       </c>
       <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="G23" s="14">
+        <v>16</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>

</xml_diff>